<commit_message>
NhamCT thêm file mẫu báo cáo
</commit_message>
<xml_diff>
--- a/Kế hoạch thực tập-TTNT45K_02.xlsx
+++ b/Kế hoạch thực tập-TTNT45K_02.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DUE\COURSES\MIS2010. Thực tập nhận thức\Hè 2021\Projects\TTNT45K_02\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
   </bookViews>
@@ -232,7 +237,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -694,7 +699,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -704,10 +709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -738,7 +742,9 @@
       <c r="E2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="23"/>
+      <c r="F2" s="23">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">

</xml_diff>